<commit_message>
add functional group analysis
</commit_message>
<xml_diff>
--- a/Datas/SOM++_clustercenters.xlsx
+++ b/Datas/SOM++_clustercenters.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,22 +475,22 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -498,68 +498,91 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E3" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="G4" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>13</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>